<commit_message>
Correções em mapas de apropriação do IQ.
</commit_message>
<xml_diff>
--- a/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_REC.XLSX
+++ b/outputs/sisaprophelper#autoaprop/autoapropxlsx/IQ_REC.XLSX
@@ -153,6 +153,9 @@
     <t>GERSON R.DOS S.JUNIOR</t>
   </si>
   <si>
+    <t>JOEL FELIPE</t>
+  </si>
+  <si>
     <t>ANDERSON CLEMENTINO DA SILVA</t>
   </si>
   <si>
@@ -237,12 +240,12 @@
     <t> </t>
   </si>
   <si>
-    <t> </t>
-  </si>
-  <si>
     <t>2374</t>
   </si>
   <si>
+    <t>2561</t>
+  </si>
+  <si>
     <t>3241</t>
   </si>
   <si>
@@ -256,9 +259,6 @@
   </si>
   <si>
     <t>4277</t>
-  </si>
-  <si>
-    <t> </t>
   </si>
   <si>
     <t> </t>

</xml_diff>